<commit_message>
🔨 Primeros datos de aire (5min)
</commit_message>
<xml_diff>
--- a/aplicaciones/procesador/datos/Mapa 7ma - Datos.xlsx
+++ b/aplicaciones/procesador/datos/Mapa 7ma - Datos.xlsx
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="356">
   <si>
     <t>edificio los venados</t>
   </si>
@@ -518,10 +518,7 @@
     <t>puntoRuido</t>
   </si>
   <si>
-    <t>pm25 puntos fijos</t>
-  </si>
-  <si>
-    <t>ebc puntos fijos</t>
+    <t>idAire</t>
   </si>
   <si>
     <t xml:space="preserve">Txt 15 minutos </t>
@@ -2399,19 +2396,18 @@
     <col customWidth="1" min="5" max="5" width="12.38"/>
     <col customWidth="1" min="6" max="6" width="11.5"/>
     <col customWidth="1" min="7" max="7" width="15.25"/>
-    <col customWidth="1" min="8" max="8" width="14.13"/>
-    <col customWidth="1" min="9" max="9" width="13.25"/>
-    <col customWidth="1" min="10" max="10" width="10.0"/>
-    <col customWidth="1" min="11" max="11" width="10.5"/>
-    <col customWidth="1" min="12" max="12" width="8.63"/>
-    <col customWidth="1" min="13" max="13" width="13.38"/>
-    <col customWidth="1" min="14" max="14" width="15.38"/>
-    <col customWidth="1" min="15" max="15" width="15.75"/>
-    <col customWidth="1" min="16" max="16" width="8.5"/>
-    <col customWidth="1" min="17" max="17" width="8.0"/>
-    <col customWidth="1" min="18" max="18" width="7.0"/>
-    <col customWidth="1" min="19" max="19" width="40.88"/>
-    <col customWidth="1" min="20" max="20" width="20.88"/>
+    <col customWidth="1" min="8" max="8" width="13.25"/>
+    <col customWidth="1" min="9" max="9" width="10.0"/>
+    <col customWidth="1" min="10" max="10" width="10.5"/>
+    <col customWidth="1" min="11" max="11" width="8.63"/>
+    <col customWidth="1" min="12" max="12" width="13.38"/>
+    <col customWidth="1" min="13" max="13" width="15.38"/>
+    <col customWidth="1" min="14" max="14" width="15.75"/>
+    <col customWidth="1" min="15" max="15" width="8.5"/>
+    <col customWidth="1" min="16" max="16" width="8.0"/>
+    <col customWidth="1" min="17" max="17" width="7.0"/>
+    <col customWidth="1" min="18" max="18" width="40.88"/>
+    <col customWidth="1" min="19" max="19" width="20.88"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2472,16 +2468,13 @@
       <c r="S1" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="T1" s="3" t="s">
-        <v>162</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
         <v>1.0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C2" s="22">
         <v>4.59779533018865</v>
@@ -2490,13 +2483,13 @@
         <v>-74.0756536703986</v>
       </c>
       <c r="E2" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="M2" s="24" t="s">
         <v>164</v>
       </c>
       <c r="N2" s="24" t="s">
         <v>165</v>
-      </c>
-      <c r="O2" s="24" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="3">
@@ -2504,7 +2497,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C3" s="22">
         <v>4.601444</v>
@@ -2513,29 +2506,29 @@
         <v>-74.073396</v>
       </c>
       <c r="E3" s="26"/>
-      <c r="K3" s="1" t="s">
+      <c r="J3" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1" t="s">
+      <c r="N3" s="1"/>
+      <c r="O3" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="O3" s="1"/>
-      <c r="P3" s="24" t="s">
+      <c r="R3" s="27" t="s">
         <v>170</v>
       </c>
-      <c r="S3" s="27" t="s">
-        <v>171</v>
-      </c>
-      <c r="T3" s="27"/>
+      <c r="S3" s="27"/>
     </row>
     <row r="4">
       <c r="A4" s="1">
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C4" s="22">
         <v>4.605297</v>
@@ -2544,19 +2537,19 @@
         <v>-74.071588</v>
       </c>
       <c r="E4" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>173</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>175</v>
-      </c>
+      <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="R4" s="1" t="s">
-        <v>176</v>
+      <c r="Q4" s="1" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="5">
@@ -2564,7 +2557,7 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C5" s="22">
         <v>4.61134</v>
@@ -2573,28 +2566,28 @@
         <v>-74.069874</v>
       </c>
       <c r="E5" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="I5" s="24" t="s">
         <v>178</v>
       </c>
-      <c r="J5" s="24" t="s">
-        <v>179</v>
-      </c>
+      <c r="J5" s="24"/>
       <c r="K5" s="24"/>
       <c r="L5" s="24"/>
       <c r="M5" s="24"/>
       <c r="N5" s="24"/>
       <c r="O5" s="24"/>
-      <c r="P5" s="24"/>
-      <c r="S5" s="1" t="s">
+      <c r="R5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="T5" s="1"/>
+      <c r="S5" s="1"/>
     </row>
     <row r="6">
       <c r="A6" s="1">
         <v>5.0</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C6" s="22">
         <v>4.618599</v>
@@ -2603,34 +2596,34 @@
         <v>-74.068069</v>
       </c>
       <c r="E6" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="I6" s="24" t="s">
         <v>178</v>
       </c>
-      <c r="J6" s="24" t="s">
-        <v>179</v>
-      </c>
+      <c r="J6" s="24"/>
       <c r="K6" s="24"/>
       <c r="L6" s="24"/>
       <c r="M6" s="24"/>
       <c r="N6" s="24"/>
       <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
+      <c r="P6" s="1" t="s">
+        <v>180</v>
+      </c>
       <c r="Q6" s="1" t="s">
         <v>181</v>
       </c>
       <c r="R6" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="S6" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="T6" s="1"/>
+      <c r="S6" s="1"/>
     </row>
     <row r="7">
       <c r="A7" s="25">
         <v>6.0</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C7" s="22">
         <v>4.62475</v>
@@ -2639,24 +2632,24 @@
         <v>-74.066423</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F7" s="29">
         <v>1.0</v>
       </c>
-      <c r="J7" s="24" t="s">
-        <v>179</v>
-      </c>
+      <c r="I7" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="J7" s="24"/>
       <c r="K7" s="24"/>
       <c r="L7" s="24"/>
       <c r="M7" s="24"/>
       <c r="N7" s="24"/>
       <c r="O7" s="24"/>
-      <c r="P7" s="24"/>
-      <c r="S7" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="T7" s="1"/>
+      <c r="R7" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="S7" s="1"/>
     </row>
     <row r="8">
       <c r="A8" s="1">
@@ -2672,30 +2665,30 @@
         <v>-74.064257</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>185</v>
-      </c>
-      <c r="J8" s="24" t="s">
-        <v>179</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="I8" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="J8" s="24"/>
       <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24" t="s">
-        <v>187</v>
-      </c>
+      <c r="L8" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="M8" s="24"/>
       <c r="N8" s="24"/>
       <c r="O8" s="24"/>
-      <c r="P8" s="24"/>
-      <c r="S8" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="T8" s="1"/>
+      <c r="R8" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="S8" s="1"/>
     </row>
     <row r="9">
       <c r="A9" s="25">
         <v>8.0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C9" s="22">
         <v>4.6282521</v>
@@ -2704,28 +2697,28 @@
         <v>-74.0670904</v>
       </c>
       <c r="E9" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>190</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="K9" s="1"/>
+      <c r="L9" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1" t="s">
-        <v>193</v>
-      </c>
+      <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
     </row>
     <row r="10">
       <c r="A10" s="1">
         <v>9.0</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C10" s="22">
         <v>4.639489</v>
@@ -2734,37 +2727,34 @@
         <v>-74.062897</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F10" s="29">
         <v>2.0</v>
       </c>
       <c r="G10" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="H10" s="30" t="s">
-        <v>196</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1" t="s">
+      <c r="M10" s="24" t="s">
         <v>197</v>
       </c>
-      <c r="N10" s="24" t="s">
-        <v>198</v>
-      </c>
+      <c r="N10" s="24"/>
       <c r="O10" s="24"/>
-      <c r="P10" s="24"/>
     </row>
     <row r="11">
       <c r="A11" s="25">
         <v>10.0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C11" s="22">
         <v>4.641975</v>
@@ -2773,27 +2763,27 @@
         <v>-74.062267</v>
       </c>
       <c r="E11" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="H11" s="24" t="s">
         <v>200</v>
       </c>
-      <c r="I11" s="24" t="s">
-        <v>201</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>191</v>
-      </c>
+      <c r="I11" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
     </row>
     <row r="12">
       <c r="A12" s="1">
         <v>11.0</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C12" s="22">
         <v>4.645357</v>
@@ -2802,26 +2792,26 @@
         <v>-74.061291</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F12" s="29">
         <v>3.0</v>
       </c>
       <c r="G12" s="30" t="s">
+        <v>203</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="H12" s="30" t="s">
-        <v>204</v>
-      </c>
       <c r="I12" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>191</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
+      <c r="M12" s="1" t="s">
+        <v>205</v>
+      </c>
       <c r="N12" s="1" t="s">
         <v>206</v>
       </c>
@@ -2837,17 +2827,14 @@
       <c r="R12" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="S12" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="T12" s="1"/>
+      <c r="S12" s="1"/>
     </row>
     <row r="13">
       <c r="A13" s="25">
         <v>12.0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C13" s="22">
         <v>4.6507</v>
@@ -2856,21 +2843,21 @@
         <v>-74.05822</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>213</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>191</v>
-      </c>
+        <v>212</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
+      <c r="O13" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="P13" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="14">
@@ -2878,7 +2865,7 @@
         <v>13.0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C14" s="22">
         <v>4.652758</v>
@@ -2887,19 +2874,19 @@
         <v>-74.056551</v>
       </c>
       <c r="E14" s="28" t="s">
-        <v>185</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>191</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1" t="s">
-        <v>209</v>
+      <c r="P14" s="1" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="15">
@@ -2907,7 +2894,7 @@
         <v>14.0</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C15" s="22">
         <v>4.65487400724876</v>
@@ -2916,31 +2903,31 @@
         <v>-74.0554333681108</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>191</v>
-      </c>
+        <v>216</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="S15" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="T15" s="1"/>
+      <c r="P15" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="S15" s="1"/>
     </row>
     <row r="16">
       <c r="A16" s="1">
         <v>15.0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C16" s="22">
         <v>4.65671780613089</v>
@@ -2949,24 +2936,24 @@
         <v>-74.0543665308446</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>220</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>191</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
     </row>
     <row r="17">
       <c r="A17" s="25">
         <v>16.0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C17" s="22">
         <v>4.65869671902702</v>
@@ -2975,26 +2962,26 @@
         <v>-74.0527981659214</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>191</v>
-      </c>
+        <v>216</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="24" t="s">
-        <v>222</v>
-      </c>
+      <c r="M17" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="N17" s="24"/>
       <c r="O17" s="24"/>
-      <c r="P17" s="24"/>
     </row>
     <row r="18">
       <c r="A18" s="1">
         <v>17.0</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C18" s="22">
         <v>4.66306901162081</v>
@@ -3003,39 +2990,36 @@
         <v>-74.0486994996409</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G18" s="30" t="s">
+        <v>223</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="H18" s="30" t="s">
-        <v>224</v>
-      </c>
       <c r="I18" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="J18" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1" t="s">
-        <v>226</v>
-      </c>
+      <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
-      <c r="S18" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="T18" s="1"/>
+      <c r="R18" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="S18" s="1"/>
     </row>
     <row r="19">
       <c r="A19" s="25">
         <v>18.0</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C19" s="22">
         <v>4.66516565077258</v>
@@ -3044,23 +3028,23 @@
         <v>-74.0468160288417</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F19" s="29">
         <v>4.0</v>
       </c>
-      <c r="J19" s="1" t="s">
-        <v>191</v>
-      </c>
+      <c r="I19" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="J19" s="1"/>
       <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
     </row>
     <row r="20">
       <c r="A20" s="1">
         <v>19.0</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C20" s="22">
         <v>4.67138521212362</v>
@@ -3069,28 +3053,28 @@
         <v>-74.0438000439461</v>
       </c>
       <c r="E20" s="23" t="s">
-        <v>230</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>191</v>
-      </c>
+        <v>229</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="S20" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="T20" s="1"/>
+      <c r="R20" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="S20" s="1"/>
     </row>
     <row r="21">
       <c r="A21" s="25">
         <v>20.0</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C21" s="22">
         <v>4.67447260123109</v>
@@ -3099,28 +3083,28 @@
         <v>-74.0417018437693</v>
       </c>
       <c r="E21" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="I21" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="J21" s="1" t="s">
-        <v>191</v>
-      </c>
+      <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="S21" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="T21" s="1"/>
+      <c r="R21" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="S21" s="1"/>
     </row>
     <row r="22">
       <c r="A22" s="1">
         <v>21.0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C22" s="22">
         <v>4.67985737530602</v>
@@ -3129,22 +3113,22 @@
         <v>-74.0382125791768</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>230</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>191</v>
-      </c>
+        <v>229</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
+      <c r="P22" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="Q22" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="R22" s="1" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="23">
@@ -3152,7 +3136,7 @@
         <v>22.0</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C23" s="22">
         <v>4.6851414298036</v>
@@ -3161,37 +3145,34 @@
         <v>-74.0356604991655</v>
       </c>
       <c r="E23" s="28" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F23" s="29">
         <v>5.0</v>
       </c>
       <c r="G23" s="30" t="s">
+        <v>237</v>
+      </c>
+      <c r="I23" s="24" t="s">
         <v>238</v>
       </c>
-      <c r="H23" s="30" t="s">
-        <v>238</v>
-      </c>
-      <c r="J23" s="24" t="s">
-        <v>239</v>
-      </c>
+      <c r="J23" s="24"/>
       <c r="K23" s="24"/>
       <c r="L23" s="24"/>
       <c r="M23" s="24"/>
       <c r="N23" s="24"/>
       <c r="O23" s="24"/>
-      <c r="P23" s="24"/>
-      <c r="S23" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="T23" s="1"/>
+      <c r="R23" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="S23" s="1"/>
     </row>
     <row r="24">
       <c r="A24" s="1">
         <v>23.0</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C24" s="22">
         <v>4.69366275843025</v>
@@ -3200,28 +3181,28 @@
         <v>-74.0332252216773</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>242</v>
-      </c>
-      <c r="J24" s="24" t="s">
-        <v>239</v>
-      </c>
+        <v>241</v>
+      </c>
+      <c r="I24" s="24" t="s">
+        <v>238</v>
+      </c>
+      <c r="J24" s="24"/>
       <c r="K24" s="24"/>
       <c r="L24" s="24"/>
       <c r="M24" s="24"/>
       <c r="N24" s="24"/>
       <c r="O24" s="24"/>
-      <c r="P24" s="24"/>
-      <c r="S24" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="T24" s="1"/>
+      <c r="R24" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="S24" s="1"/>
     </row>
     <row r="25">
       <c r="A25" s="25">
         <v>24.0</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C25" s="22">
         <v>4.70213634871971</v>
@@ -3230,24 +3211,24 @@
         <v>-74.0285922020549</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>203</v>
-      </c>
-      <c r="J25" s="24" t="s">
-        <v>239</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="I25" s="24" t="s">
+        <v>238</v>
+      </c>
+      <c r="J25" s="24"/>
       <c r="K25" s="24"/>
       <c r="L25" s="24"/>
       <c r="M25" s="24"/>
       <c r="N25" s="24"/>
       <c r="O25" s="24"/>
-      <c r="P25" s="24"/>
     </row>
     <row r="26">
       <c r="A26" s="1">
         <v>25.0</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C26" s="22">
         <v>4.71168163739051</v>
@@ -3256,33 +3237,30 @@
         <v>-74.029166381959</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F26" s="29">
         <v>6.0</v>
       </c>
       <c r="G26" s="30" t="s">
-        <v>246</v>
-      </c>
-      <c r="H26" s="30" t="s">
-        <v>246</v>
-      </c>
-      <c r="J26" s="24" t="s">
-        <v>239</v>
-      </c>
+        <v>245</v>
+      </c>
+      <c r="I26" s="24" t="s">
+        <v>238</v>
+      </c>
+      <c r="J26" s="24"/>
       <c r="K26" s="24"/>
       <c r="L26" s="24"/>
       <c r="M26" s="24"/>
       <c r="N26" s="24"/>
       <c r="O26" s="24"/>
-      <c r="P26" s="24"/>
     </row>
     <row r="27">
       <c r="A27" s="25">
         <v>26.0</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C27" s="22">
         <v>4.71618941013746</v>
@@ -3291,30 +3269,30 @@
         <v>-74.028746372056</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>213</v>
-      </c>
-      <c r="J27" s="24" t="s">
-        <v>239</v>
-      </c>
+        <v>212</v>
+      </c>
+      <c r="I27" s="24" t="s">
+        <v>238</v>
+      </c>
+      <c r="J27" s="24"/>
       <c r="K27" s="24"/>
       <c r="L27" s="24"/>
-      <c r="M27" s="24"/>
-      <c r="N27" s="24" t="s">
+      <c r="M27" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="N27" s="24"/>
+      <c r="O27" s="24"/>
+      <c r="R27" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="O27" s="24"/>
-      <c r="P27" s="24"/>
-      <c r="S27" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="T27" s="1"/>
+      <c r="S27" s="1"/>
     </row>
     <row r="28">
       <c r="A28" s="1">
         <v>27.0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C28" s="22">
         <v>4.72271112809495</v>
@@ -3323,24 +3301,24 @@
         <v>-74.0261459774934</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>251</v>
-      </c>
-      <c r="J28" s="24" t="s">
-        <v>239</v>
-      </c>
+        <v>250</v>
+      </c>
+      <c r="I28" s="24" t="s">
+        <v>238</v>
+      </c>
+      <c r="J28" s="24"/>
       <c r="K28" s="24"/>
       <c r="L28" s="24"/>
       <c r="M28" s="24"/>
       <c r="N28" s="24"/>
       <c r="O28" s="24"/>
-      <c r="P28" s="24"/>
     </row>
     <row r="29">
       <c r="A29" s="25">
         <v>28.0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C29" s="22">
         <v>4.72561860463364</v>
@@ -3349,19 +3327,19 @@
         <v>-74.0248846037107</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>195</v>
-      </c>
-      <c r="J29" s="24" t="s">
-        <v>239</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="I29" s="24" t="s">
+        <v>238</v>
+      </c>
+      <c r="J29" s="24"/>
       <c r="K29" s="24"/>
       <c r="L29" s="24"/>
       <c r="M29" s="24"/>
       <c r="N29" s="24"/>
       <c r="O29" s="24"/>
-      <c r="P29" s="24"/>
-      <c r="R29" s="1" t="s">
-        <v>253</v>
+      <c r="Q29" s="1" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="30">
@@ -3369,7 +3347,7 @@
         <v>29.0</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C30" s="22">
         <v>4.72759203191308</v>
@@ -3378,27 +3356,27 @@
         <v>-74.0246188787511</v>
       </c>
       <c r="E30" s="23" t="s">
-        <v>220</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="J30" s="24" t="s">
-        <v>239</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="I30" s="24" t="s">
+        <v>238</v>
+      </c>
+      <c r="J30" s="24"/>
       <c r="K30" s="24"/>
       <c r="L30" s="24"/>
       <c r="M30" s="24"/>
       <c r="N30" s="24"/>
       <c r="O30" s="24"/>
-      <c r="P30" s="24"/>
     </row>
     <row r="31">
       <c r="A31" s="25">
         <v>30.0</v>
       </c>
       <c r="B31" s="29" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C31" s="22">
         <v>4.73504479371492</v>
@@ -3407,37 +3385,34 @@
         <v>-74.0243405599811</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G31" s="30" t="s">
+        <v>256</v>
+      </c>
+      <c r="H31" s="24" t="s">
         <v>257</v>
       </c>
-      <c r="H31" s="30" t="s">
-        <v>257</v>
-      </c>
       <c r="I31" s="24" t="s">
+        <v>238</v>
+      </c>
+      <c r="J31" s="24"/>
+      <c r="K31" s="24"/>
+      <c r="L31" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="J31" s="24" t="s">
-        <v>239</v>
-      </c>
-      <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
       <c r="M31" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="N31" s="1" t="s">
-        <v>260</v>
-      </c>
+      <c r="N31" s="1"/>
       <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
     </row>
     <row r="32">
       <c r="A32" s="1">
         <v>31.0</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C32" s="22">
         <v>4.73928285919624</v>
@@ -3446,21 +3421,21 @@
         <v>-74.0227685844767</v>
       </c>
       <c r="E32" s="23" t="s">
-        <v>220</v>
-      </c>
-      <c r="M32" s="1" t="s">
-        <v>262</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="M32" s="1"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
     </row>
     <row r="33">
       <c r="A33" s="25">
         <v>32.0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C33" s="22">
         <v>4.74104500723192</v>
@@ -3469,22 +3444,22 @@
         <v>-74.0223245655917</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>173</v>
-      </c>
-      <c r="I33" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="R33" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="S33" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="T33" s="1"/>
+      <c r="S33" s="1"/>
     </row>
     <row r="34">
       <c r="A34" s="1">
         <v>33.0</v>
       </c>
       <c r="B34" s="29" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C34" s="22">
         <v>4.74704550134667</v>
@@ -3493,26 +3468,23 @@
         <v>-74.0226372775582</v>
       </c>
       <c r="E34" s="28" t="s">
+        <v>266</v>
+      </c>
+      <c r="G34" s="30" t="s">
         <v>267</v>
       </c>
-      <c r="G34" s="30" t="s">
+      <c r="J34" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="H34" s="30" t="s">
-        <v>268</v>
-      </c>
-      <c r="K34" s="1" t="s">
+      <c r="K34" s="1"/>
+      <c r="L34" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1" t="s">
-        <v>270</v>
-      </c>
+      <c r="M34" s="1"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
-      <c r="Q34" s="1" t="s">
-        <v>271</v>
+      <c r="P34" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="35">
@@ -3520,7 +3492,7 @@
         <v>34.0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C35" s="22">
         <v>4.75396347261005</v>
@@ -3529,10 +3501,10 @@
         <v>-74.0244240661433</v>
       </c>
       <c r="E35" s="28" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q35" s="1" t="s">
         <v>273</v>
-      </c>
-      <c r="R35" s="1" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="36">
@@ -3540,7 +3512,7 @@
         <v>35.0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C36" s="22">
         <v>4.75617544590708</v>
@@ -3549,19 +3521,19 @@
         <v>-74.0246792916686</v>
       </c>
       <c r="E36" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="S36" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="T36" s="1"/>
+        <v>229</v>
+      </c>
+      <c r="R36" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="S36" s="1"/>
     </row>
     <row r="37">
       <c r="A37" s="25">
         <v>36.0</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C37" s="22">
         <v>4.76052434895997</v>
@@ -3570,19 +3542,19 @@
         <v>-74.0263419552712</v>
       </c>
       <c r="E37" s="28" t="s">
-        <v>213</v>
-      </c>
-      <c r="S37" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="T37" s="1"/>
+        <v>212</v>
+      </c>
+      <c r="R37" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="S37" s="1"/>
     </row>
     <row r="38">
       <c r="A38" s="1">
         <v>37.0</v>
       </c>
       <c r="B38" s="29" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C38" s="22">
         <v>4.76566235110988</v>
@@ -3591,16 +3563,13 @@
         <v>-74.027549403371</v>
       </c>
       <c r="E38" s="28" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G38" s="30" t="s">
+        <v>279</v>
+      </c>
+      <c r="O38" s="1" t="s">
         <v>280</v>
-      </c>
-      <c r="H38" s="30" t="s">
-        <v>280</v>
-      </c>
-      <c r="P38" s="1" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="39">
@@ -3608,7 +3577,7 @@
         <v>38.0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C39" s="22">
         <v>4.7689779473818</v>
@@ -3617,7 +3586,7 @@
         <v>-74.0273381986581</v>
       </c>
       <c r="E39" s="28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="40">
@@ -3625,7 +3594,7 @@
         <v>39.0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C40" s="22">
         <v>4.76966052997788</v>
@@ -3634,19 +3603,19 @@
         <v>-74.0270269840824</v>
       </c>
       <c r="E40" s="28" t="s">
+        <v>284</v>
+      </c>
+      <c r="R40" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="S40" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="T40" s="1"/>
+      <c r="S40" s="1"/>
     </row>
     <row r="41">
       <c r="A41" s="25">
         <v>40.0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C41" s="22">
         <v>4.7771118817951</v>
@@ -3655,19 +3624,19 @@
         <v>-74.0260495949368</v>
       </c>
       <c r="E41" s="28" t="s">
+        <v>287</v>
+      </c>
+      <c r="R41" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="S41" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="T41" s="1"/>
+      <c r="S41" s="1"/>
     </row>
     <row r="42">
       <c r="A42" s="1">
         <v>41.0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C42" s="22">
         <v>4.79861514914944</v>
@@ -3676,7 +3645,7 @@
         <v>-74.0307002114146</v>
       </c>
       <c r="E42" s="28" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -3704,21 +3673,21 @@
         <v>143</v>
       </c>
       <c r="B1" s="31" t="s">
+        <v>291</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>292</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B2" s="24" t="s">
+        <v>293</v>
+      </c>
+      <c r="C2" s="32" t="s">
         <v>294</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>295</v>
       </c>
       <c r="D2" s="32"/>
       <c r="E2" s="32"/>
@@ -3726,13 +3695,13 @@
     </row>
     <row r="3">
       <c r="A3" s="24" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D3" s="33"/>
       <c r="E3" s="33"/>
@@ -3750,13 +3719,13 @@
     </row>
     <row r="4">
       <c r="A4" s="24" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
@@ -3769,354 +3738,354 @@
     </row>
     <row r="5">
       <c r="A5" s="24" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B5" s="24" t="s">
+        <v>297</v>
+      </c>
+      <c r="C5" s="32" t="s">
         <v>298</v>
-      </c>
-      <c r="C5" s="32" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="24" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="24" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="24" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B8" s="24" t="s">
+        <v>301</v>
+      </c>
+      <c r="C8" s="32" t="s">
         <v>302</v>
-      </c>
-      <c r="C8" s="32" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="24" t="s">
+        <v>303</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>301</v>
+      </c>
+      <c r="C9" s="32" t="s">
         <v>304</v>
-      </c>
-      <c r="B9" s="24" t="s">
-        <v>302</v>
-      </c>
-      <c r="C9" s="32" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="24" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B10" s="24" t="s">
+        <v>305</v>
+      </c>
+      <c r="C10" s="32" t="s">
         <v>306</v>
-      </c>
-      <c r="C10" s="32" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="24" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="24" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="24" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="24" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="24" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="24" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B18" s="24" t="s">
+        <v>314</v>
+      </c>
+      <c r="C18" s="32" t="s">
         <v>315</v>
-      </c>
-      <c r="C18" s="32" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="24" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C19" s="32" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="24" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C20" s="32" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="24" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C21" s="32" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="24" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C22" s="32" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="24" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C23" s="32" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="24" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B24" s="24" t="s">
         <v>147</v>
       </c>
       <c r="C24" s="32" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B25" s="24" t="s">
         <v>147</v>
       </c>
       <c r="C25" s="32" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B26" s="24" t="s">
         <v>147</v>
       </c>
       <c r="C26" s="32" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B27" s="24" t="s">
         <v>147</v>
       </c>
       <c r="C27" s="32" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="24" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B28" s="24" t="s">
         <v>147</v>
       </c>
       <c r="C28" s="32" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="24" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B29" s="24" t="s">
         <v>147</v>
       </c>
       <c r="C29" s="32" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="24" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B30" s="24" t="s">
         <v>147</v>
       </c>
       <c r="C30" s="32" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B31" s="24" t="s">
+        <v>328</v>
+      </c>
+      <c r="C31" s="32" t="s">
         <v>329</v>
-      </c>
-      <c r="C31" s="32" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="24" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C32" s="32" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="24" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B33" s="24" t="s">
         <v>119</v>
       </c>
       <c r="C33" s="32" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="24" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B34" s="24" t="s">
         <v>119</v>
       </c>
       <c r="C34" s="32" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B35" s="24" t="s">
         <v>119</v>
       </c>
       <c r="C35" s="32" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="24" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B36" s="24" t="s">
         <v>119</v>
       </c>
       <c r="C36" s="32" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="37">
@@ -8001,196 +7970,196 @@
         <v>143</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>338</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>121</v>
       </c>
       <c r="D2" s="36"/>
       <c r="E2" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>123</v>
       </c>
       <c r="D3" s="36"/>
       <c r="E3" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>125</v>
       </c>
       <c r="D4" s="36"/>
       <c r="E4" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>81</v>
       </c>
       <c r="D5" s="36"/>
       <c r="E5" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>129</v>
       </c>
       <c r="D6" s="36"/>
       <c r="E6" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>131</v>
       </c>
       <c r="D7" s="36"/>
       <c r="E7" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>132</v>
       </c>
       <c r="D8" s="36"/>
       <c r="E8" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>134</v>
       </c>
       <c r="D9" s="36"/>
       <c r="E9" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>136</v>
       </c>
       <c r="D10" s="36"/>
       <c r="E10" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>138</v>
       </c>
       <c r="D11" s="36"/>
       <c r="E11" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>140</v>
       </c>
       <c r="D12" s="36"/>
       <c r="E12" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>142</v>
       </c>
       <c r="D13" s="36"/>
       <c r="E13" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
✅ Agregar perfiles y podcasts a puntos
</commit_message>
<xml_diff>
--- a/aplicaciones/procesador/datos/Mapa 7ma - Datos.xlsx
+++ b/aplicaciones/procesador/datos/Mapa 7ma - Datos.xlsx
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="354">
   <si>
     <t>edificio los venados</t>
   </si>
@@ -545,10 +545,10 @@
     <t>Txt Salud</t>
   </si>
   <si>
-    <t xml:space="preserve">Podcast </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Perfil </t>
+    <t>podcast</t>
+  </si>
+  <si>
+    <t>perfil</t>
   </si>
   <si>
     <t>ilustracion</t>
@@ -1095,9 +1095,6 @@
     <t>ruta archivo</t>
   </si>
   <si>
-    <t>podcast</t>
-  </si>
-  <si>
     <t>aire_ruido</t>
   </si>
   <si>
@@ -1108,9 +1105,6 @@
   </si>
   <si>
     <t>habitabilidad</t>
-  </si>
-  <si>
-    <t>perfil</t>
   </si>
   <si>
     <t>habitabilidad_1</t>
@@ -7987,14 +7981,14 @@
         <v>270</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>339</v>
+        <v>158</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>121</v>
       </c>
       <c r="D2" s="36"/>
       <c r="E2" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="3">
@@ -8002,14 +7996,14 @@
         <v>208</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>339</v>
+        <v>158</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>123</v>
       </c>
       <c r="D3" s="36"/>
       <c r="E3" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="4">
@@ -8017,14 +8011,14 @@
         <v>234</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>339</v>
+        <v>158</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>125</v>
       </c>
       <c r="D4" s="36"/>
       <c r="E4" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="5">
@@ -8032,14 +8026,14 @@
         <v>180</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>339</v>
+        <v>158</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>81</v>
       </c>
       <c r="D5" s="36"/>
       <c r="E5" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="6">
@@ -8047,29 +8041,29 @@
         <v>181</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>344</v>
+        <v>159</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>129</v>
       </c>
       <c r="D6" s="36"/>
       <c r="E6" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>344</v>
+        <v>159</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>131</v>
       </c>
       <c r="D7" s="36"/>
       <c r="E7" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="8">
@@ -8077,14 +8071,14 @@
         <v>252</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>344</v>
+        <v>159</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>132</v>
       </c>
       <c r="D8" s="36"/>
       <c r="E8" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="9">
@@ -8092,29 +8086,29 @@
         <v>209</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>344</v>
+        <v>159</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>134</v>
       </c>
       <c r="D9" s="36"/>
       <c r="E9" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>344</v>
+        <v>159</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>136</v>
       </c>
       <c r="D10" s="36"/>
       <c r="E10" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="11">
@@ -8122,14 +8116,14 @@
         <v>175</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>344</v>
+        <v>159</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>138</v>
       </c>
       <c r="D11" s="36"/>
       <c r="E11" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="12">
@@ -8137,29 +8131,29 @@
         <v>235</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>344</v>
+        <v>159</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>140</v>
       </c>
       <c r="D12" s="36"/>
       <c r="E12" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>344</v>
+        <v>159</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>142</v>
       </c>
       <c r="D13" s="36"/>
       <c r="E13" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
🤡 más ilustraciones de prueba
</commit_message>
<xml_diff>
--- a/aplicaciones/procesador/datos/Mapa 7ma - Datos.xlsx
+++ b/aplicaciones/procesador/datos/Mapa 7ma - Datos.xlsx
@@ -8,10 +8,10 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Cuatro cuadras" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="Textos" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="Elementos" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Cuatro cuadras" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Textos" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Elementos" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +25,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>Autoría desconocida</author>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0">
@@ -33,8 +33,10 @@
         <r>
           <rPr>
             <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <family val="2"/>
+            <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">sugiero invertir el orden de estos dos porque la Javeriana queda antes de la 45 yendo de sur a norte
 	-Antonia Bu
@@ -49,8 +51,10 @@
         <r>
           <rPr>
             <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <family val="2"/>
+            <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Los datos tomados son en la cll 37
 	-Antonia Bu</t>
@@ -62,8 +66,10 @@
         <r>
           <rPr>
             <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <family val="2"/>
+            <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">hay datos en la 61
 	-Antonia Bu</t>
@@ -75,8 +81,10 @@
         <r>
           <rPr>
             <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <family val="2"/>
+            <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">la 84 no existe, cambié por 84A
 	-Antonia Bu</t>
@@ -88,8 +96,10 @@
         <r>
           <rPr>
             <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <family val="2"/>
+            <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Hay datos en la 86
 	-Antonia Bu</t>
@@ -101,8 +111,10 @@
         <r>
           <rPr>
             <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <family val="2"/>
+            <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Hay datos en la 108A
 	-Antonia Bu</t>
@@ -114,8 +126,10 @@
         <r>
           <rPr>
             <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <family val="2"/>
+            <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Hay datos en la calle 132
 	-Antonia Bu</t>
@@ -127,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="354">
   <si>
     <t xml:space="preserve">edificio los venados</t>
   </si>
@@ -625,6 +639,9 @@
   </si>
   <si>
     <t xml:space="preserve">tfp1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plaza_de_bolivar</t>
   </si>
   <si>
     <t xml:space="preserve">Avenida Jiménez</t>
@@ -1203,7 +1220,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1228,7 +1245,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
@@ -1236,15 +1253,10 @@
     <font>
       <b val="true"/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -1252,19 +1264,6 @@
       <name val="&quot;Google Sans&quot;"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="9"/>
@@ -1283,7 +1282,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFFF6D01"/>
         <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
@@ -1319,7 +1318,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FF46BDC6"/>
         <bgColor rgb="FF339966"/>
       </patternFill>
     </fill>
@@ -1391,7 +1390,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1484,11 +1483,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1500,10 +1499,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1512,7 +1507,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1520,23 +1515,19 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1612,180 +1603,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
-  <a:themeElements>
-    <a:clrScheme name="Sheets">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="ffffff"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4285f4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ea4335"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="fbbc04"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="34a853"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="ff6d01"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="46bdc6"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="1155cc"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="1155cc"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Sheets">
-      <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:cs typeface="Arial" pitchFamily="0" charset="1"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:cs typeface="Arial" pitchFamily="0" charset="1"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
@@ -1799,7 +1618,7 @@
       <selection pane="bottomRight" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.65234375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.25"/>
@@ -1808,19 +1627,19 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="29.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="25.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="14.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="18.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="18.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="18.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="27.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="16.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="27.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="13.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="15.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="15.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="17.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="26.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="32.13"/>
@@ -2590,38 +2409,38 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="Q36" activeCellId="0" sqref="Q36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="R2" activeCellId="0" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.65234375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="8.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="15.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="8.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="8.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="40.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="40.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="20.88"/>
   </cols>
   <sheetData>
@@ -2706,13 +2525,16 @@
       <c r="N2" s="25" t="s">
         <v>165</v>
       </c>
+      <c r="R2" s="0" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C3" s="23" t="n">
         <v>4.601444</v>
@@ -2720,30 +2542,30 @@
       <c r="D3" s="23" t="n">
         <v>-74.073396</v>
       </c>
-      <c r="E3" s="27"/>
+      <c r="E3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="25" t="s">
-        <v>169</v>
-      </c>
-      <c r="R3" s="28" t="s">
         <v>170</v>
       </c>
-      <c r="S3" s="28"/>
+      <c r="R3" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="S3" s="27"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C4" s="23" t="n">
         <v>4.605297</v>
@@ -2752,19 +2574,19 @@
         <v>-74.071588</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="Q4" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2772,7 +2594,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C5" s="23" t="n">
         <v>4.61134</v>
@@ -2781,10 +2603,10 @@
         <v>-74.069874</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I5" s="25" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="J5" s="25"/>
       <c r="K5" s="25"/>
@@ -2802,7 +2624,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C6" s="23" t="n">
         <v>4.618599</v>
@@ -2811,10 +2633,10 @@
         <v>-74.068069</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I6" s="25" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="J6" s="25"/>
       <c r="K6" s="25"/>
@@ -2823,13 +2645,13 @@
       <c r="N6" s="25"/>
       <c r="O6" s="25"/>
       <c r="P6" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="S6" s="1"/>
     </row>
@@ -2837,8 +2659,8 @@
       <c r="A7" s="26" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="29" t="s">
-        <v>183</v>
+      <c r="B7" s="28" t="s">
+        <v>184</v>
       </c>
       <c r="C7" s="23" t="n">
         <v>4.62475</v>
@@ -2847,13 +2669,13 @@
         <v>-74.066423</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>184</v>
-      </c>
-      <c r="F7" s="29" t="n">
+        <v>185</v>
+      </c>
+      <c r="F7" s="28" t="n">
         <v>1</v>
       </c>
       <c r="I7" s="25" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="J7" s="25"/>
       <c r="K7" s="25"/>
@@ -2862,7 +2684,7 @@
       <c r="N7" s="25"/>
       <c r="O7" s="25"/>
       <c r="R7" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="S7" s="1"/>
     </row>
@@ -2880,21 +2702,21 @@
         <v>-74.064257</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="I8" s="25" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="J8" s="25"/>
       <c r="K8" s="25"/>
       <c r="L8" s="25" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="M8" s="25"/>
       <c r="N8" s="25"/>
       <c r="O8" s="25"/>
       <c r="R8" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="S8" s="1"/>
     </row>
@@ -2903,7 +2725,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C9" s="23" t="n">
         <v>4.6282521</v>
@@ -2912,17 +2734,17 @@
         <v>-74.0670904</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -2932,8 +2754,8 @@
       <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="29" t="s">
-        <v>193</v>
+      <c r="B10" s="28" t="s">
+        <v>194</v>
       </c>
       <c r="C10" s="23" t="n">
         <v>4.639489</v>
@@ -2942,24 +2764,24 @@
         <v>-74.062897</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>194</v>
-      </c>
-      <c r="F10" s="29" t="n">
+        <v>195</v>
+      </c>
+      <c r="F10" s="28" t="n">
         <v>2</v>
       </c>
-      <c r="G10" s="29" t="s">
-        <v>195</v>
+      <c r="G10" s="28" t="s">
+        <v>196</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="M10" s="25" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="N10" s="25"/>
       <c r="O10" s="25"/>
@@ -2969,7 +2791,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C11" s="23" t="n">
         <v>4.641975</v>
@@ -2978,13 +2800,13 @@
         <v>-74.062267</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="H11" s="25" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -2997,8 +2819,8 @@
       <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="29" t="s">
-        <v>201</v>
+      <c r="B12" s="28" t="s">
+        <v>202</v>
       </c>
       <c r="C12" s="23" t="n">
         <v>4.645357</v>
@@ -3007,40 +2829,40 @@
         <v>-74.061291</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>202</v>
-      </c>
-      <c r="F12" s="29" t="n">
+        <v>203</v>
+      </c>
+      <c r="F12" s="28" t="n">
         <v>3</v>
       </c>
-      <c r="G12" s="29" t="s">
-        <v>203</v>
+      <c r="G12" s="28" t="s">
+        <v>204</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="S12" s="1"/>
     </row>
@@ -3049,7 +2871,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C13" s="23" t="n">
         <v>4.6507</v>
@@ -3058,10 +2880,10 @@
         <v>-74.05822</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -3069,10 +2891,10 @@
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3080,7 +2902,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C14" s="23" t="n">
         <v>4.652758</v>
@@ -3089,10 +2911,10 @@
         <v>-74.056551</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -3101,7 +2923,7 @@
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3109,7 +2931,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C15" s="23" t="n">
         <v>4.65487400724876</v>
@@ -3118,10 +2940,10 @@
         <v>-74.0554333681108</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -3130,10 +2952,10 @@
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="S15" s="1"/>
     </row>
@@ -3142,7 +2964,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C16" s="23" t="n">
         <v>4.65671780613089</v>
@@ -3151,10 +2973,10 @@
         <v>-74.0543665308446</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -3168,7 +2990,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C17" s="23" t="n">
         <v>4.65869671902702</v>
@@ -3177,16 +2999,16 @@
         <v>-74.0527981659214</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="25" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="N17" s="25"/>
       <c r="O17" s="25"/>
@@ -3195,8 +3017,8 @@
       <c r="A18" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="29" t="s">
-        <v>222</v>
+      <c r="B18" s="28" t="s">
+        <v>223</v>
       </c>
       <c r="C18" s="23" t="n">
         <v>4.66306901162081</v>
@@ -3207,25 +3029,25 @@
       <c r="E18" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="G18" s="29" t="s">
-        <v>223</v>
+      <c r="G18" s="28" t="s">
+        <v>224</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
       <c r="R18" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="S18" s="1"/>
     </row>
@@ -3233,8 +3055,8 @@
       <c r="A19" s="26" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="29" t="s">
-        <v>227</v>
+      <c r="B19" s="28" t="s">
+        <v>228</v>
       </c>
       <c r="C19" s="23" t="n">
         <v>4.66516565077258</v>
@@ -3243,13 +3065,13 @@
         <v>-74.0468160288417</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>194</v>
-      </c>
-      <c r="F19" s="29" t="n">
+        <v>195</v>
+      </c>
+      <c r="F19" s="28" t="n">
         <v>4</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
@@ -3259,7 +3081,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C20" s="23" t="n">
         <v>4.67138521212362</v>
@@ -3268,10 +3090,10 @@
         <v>-74.0438000439461</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -3280,7 +3102,7 @@
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="R20" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="S20" s="1"/>
     </row>
@@ -3289,7 +3111,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C21" s="23" t="n">
         <v>4.67447260123109</v>
@@ -3298,10 +3120,10 @@
         <v>-74.0417018437693</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -3310,7 +3132,7 @@
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="R21" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="S21" s="1"/>
     </row>
@@ -3319,7 +3141,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C22" s="23" t="n">
         <v>4.67985737530602</v>
@@ -3328,10 +3150,10 @@
         <v>-74.0382125791768</v>
       </c>
       <c r="E22" s="24" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -3340,18 +3162,18 @@
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="26" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="29" t="s">
-        <v>236</v>
+      <c r="B23" s="28" t="s">
+        <v>237</v>
       </c>
       <c r="C23" s="23" t="n">
         <v>4.6851414298036</v>
@@ -3360,16 +3182,16 @@
         <v>-74.0356604991655</v>
       </c>
       <c r="E23" s="24" t="s">
-        <v>199</v>
-      </c>
-      <c r="F23" s="29" t="n">
+        <v>200</v>
+      </c>
+      <c r="F23" s="28" t="n">
         <v>5</v>
       </c>
-      <c r="G23" s="29" t="s">
-        <v>237</v>
+      <c r="G23" s="28" t="s">
+        <v>238</v>
       </c>
       <c r="I23" s="25" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J23" s="25"/>
       <c r="K23" s="25"/>
@@ -3378,7 +3200,7 @@
       <c r="N23" s="25"/>
       <c r="O23" s="25"/>
       <c r="R23" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="S23" s="1"/>
     </row>
@@ -3387,7 +3209,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C24" s="23" t="n">
         <v>4.69366275843025</v>
@@ -3396,10 +3218,10 @@
         <v>-74.0332252216773</v>
       </c>
       <c r="E24" s="24" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="I24" s="25" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J24" s="25"/>
       <c r="K24" s="25"/>
@@ -3408,7 +3230,7 @@
       <c r="N24" s="25"/>
       <c r="O24" s="25"/>
       <c r="R24" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="S24" s="1"/>
     </row>
@@ -3417,7 +3239,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C25" s="23" t="n">
         <v>4.70213634871971</v>
@@ -3426,10 +3248,10 @@
         <v>-74.0285922020549</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="I25" s="25" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J25" s="25"/>
       <c r="K25" s="25"/>
@@ -3442,8 +3264,8 @@
       <c r="A26" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="29" t="s">
-        <v>244</v>
+      <c r="B26" s="28" t="s">
+        <v>245</v>
       </c>
       <c r="C26" s="23" t="n">
         <v>4.71168163739051</v>
@@ -3452,16 +3274,16 @@
         <v>-74.029166381959</v>
       </c>
       <c r="E26" s="24" t="s">
-        <v>184</v>
-      </c>
-      <c r="F26" s="29" t="n">
+        <v>185</v>
+      </c>
+      <c r="F26" s="28" t="n">
         <v>6</v>
       </c>
-      <c r="G26" s="29" t="s">
-        <v>245</v>
+      <c r="G26" s="28" t="s">
+        <v>246</v>
       </c>
       <c r="I26" s="25" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J26" s="25"/>
       <c r="K26" s="25"/>
@@ -3475,7 +3297,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C27" s="23" t="n">
         <v>4.71618941013746</v>
@@ -3484,21 +3306,21 @@
         <v>-74.028746372056</v>
       </c>
       <c r="E27" s="24" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="I27" s="25" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J27" s="25"/>
       <c r="K27" s="25"/>
       <c r="L27" s="25"/>
       <c r="M27" s="25" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="N27" s="25"/>
       <c r="O27" s="25"/>
       <c r="R27" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="S27" s="1"/>
     </row>
@@ -3507,7 +3329,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C28" s="23" t="n">
         <v>4.72271112809495</v>
@@ -3516,10 +3338,10 @@
         <v>-74.0261459774934</v>
       </c>
       <c r="E28" s="24" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="I28" s="25" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J28" s="25"/>
       <c r="K28" s="25"/>
@@ -3533,7 +3355,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C29" s="23" t="n">
         <v>4.72561860463364</v>
@@ -3542,10 +3364,10 @@
         <v>-74.0248846037107</v>
       </c>
       <c r="E29" s="24" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I29" s="25" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J29" s="25"/>
       <c r="K29" s="25"/>
@@ -3554,7 +3376,7 @@
       <c r="N29" s="25"/>
       <c r="O29" s="25"/>
       <c r="Q29" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3562,7 +3384,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C30" s="23" t="n">
         <v>4.72759203191308</v>
@@ -3571,13 +3393,13 @@
         <v>-74.0246188787511</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="I30" s="25" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J30" s="25"/>
       <c r="K30" s="25"/>
@@ -3590,8 +3412,8 @@
       <c r="A31" s="26" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="29" t="s">
-        <v>255</v>
+      <c r="B31" s="28" t="s">
+        <v>256</v>
       </c>
       <c r="C31" s="23" t="n">
         <v>4.73504479371492</v>
@@ -3600,24 +3422,24 @@
         <v>-74.0243405599811</v>
       </c>
       <c r="E31" s="24" t="s">
-        <v>172</v>
-      </c>
-      <c r="G31" s="29" t="s">
-        <v>256</v>
+        <v>173</v>
+      </c>
+      <c r="G31" s="28" t="s">
+        <v>257</v>
       </c>
       <c r="H31" s="25" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="I31" s="25" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J31" s="25"/>
       <c r="K31" s="25"/>
       <c r="L31" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
@@ -3627,7 +3449,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C32" s="23" t="n">
         <v>4.73928285919624</v>
@@ -3636,10 +3458,10 @@
         <v>-74.0227685844767</v>
       </c>
       <c r="E32" s="24" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
@@ -3650,7 +3472,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C33" s="23" t="n">
         <v>4.74104500723192</v>
@@ -3659,13 +3481,13 @@
         <v>-74.0223245655917</v>
       </c>
       <c r="E33" s="24" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="S33" s="1"/>
     </row>
@@ -3673,8 +3495,8 @@
       <c r="A34" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="B34" s="29" t="s">
-        <v>265</v>
+      <c r="B34" s="28" t="s">
+        <v>266</v>
       </c>
       <c r="C34" s="23" t="n">
         <v>4.74704550134667</v>
@@ -3683,23 +3505,23 @@
         <v>-74.0226372775582</v>
       </c>
       <c r="E34" s="24" t="s">
-        <v>266</v>
-      </c>
-      <c r="G34" s="29" t="s">
         <v>267</v>
       </c>
+      <c r="G34" s="28" t="s">
+        <v>268</v>
+      </c>
       <c r="J34" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="K34" s="1"/>
       <c r="L34" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
       <c r="P34" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3707,7 +3529,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C35" s="23" t="n">
         <v>4.75396347261005</v>
@@ -3716,10 +3538,10 @@
         <v>-74.0244240661433</v>
       </c>
       <c r="E35" s="24" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3727,7 +3549,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C36" s="23" t="n">
         <v>4.75617544590708</v>
@@ -3736,13 +3558,13 @@
         <v>-74.0246792916686</v>
       </c>
       <c r="E36" s="24" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q36" s="30" t="s">
-        <v>275</v>
+        <v>230</v>
+      </c>
+      <c r="Q36" s="29" t="s">
+        <v>276</v>
       </c>
       <c r="R36" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="S36" s="1"/>
     </row>
@@ -3751,7 +3573,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C37" s="23" t="n">
         <v>4.76052434895997</v>
@@ -3760,10 +3582,10 @@
         <v>-74.0263419552712</v>
       </c>
       <c r="E37" s="24" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="R37" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="S37" s="1"/>
     </row>
@@ -3771,8 +3593,8 @@
       <c r="A38" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="B38" s="29" t="s">
-        <v>279</v>
+      <c r="B38" s="28" t="s">
+        <v>280</v>
       </c>
       <c r="C38" s="23" t="n">
         <v>4.76566235110988</v>
@@ -3783,11 +3605,11 @@
       <c r="E38" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="G38" s="29" t="s">
-        <v>280</v>
+      <c r="G38" s="28" t="s">
+        <v>281</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3795,7 +3617,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C39" s="23" t="n">
         <v>4.7689779473818</v>
@@ -3804,7 +3626,7 @@
         <v>-74.0273381986581</v>
       </c>
       <c r="E39" s="24" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3812,7 +3634,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C40" s="23" t="n">
         <v>4.76966052997788</v>
@@ -3821,10 +3643,10 @@
         <v>-74.0270269840824</v>
       </c>
       <c r="E40" s="24" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="R40" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="S40" s="1"/>
     </row>
@@ -3833,7 +3655,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C41" s="23" t="n">
         <v>4.7771118817951</v>
@@ -3842,10 +3664,10 @@
         <v>-74.0260495949368</v>
       </c>
       <c r="E41" s="24" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="R41" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="S41" s="1"/>
     </row>
@@ -3854,7 +3676,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C42" s="23" t="n">
         <v>4.79861514914944</v>
@@ -3863,7 +3685,7 @@
         <v>-74.0307002114146</v>
       </c>
       <c r="E42" s="24" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -3878,7 +3700,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3888,288 +3710,288 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.65234375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="97.25"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="31" t="s">
-        <v>292</v>
+      <c r="B1" s="30" t="s">
+        <v>293</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>294</v>
-      </c>
-      <c r="C2" s="32" t="s">
         <v>295</v>
       </c>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
+      <c r="C2" s="31" t="s">
+        <v>296</v>
+      </c>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="25" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>294</v>
-      </c>
-      <c r="C3" s="32" t="s">
-        <v>296</v>
-      </c>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
+        <v>295</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>297</v>
+      </c>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="25" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>294</v>
-      </c>
-      <c r="C4" s="32" t="s">
-        <v>297</v>
-      </c>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
+        <v>295</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>298</v>
+      </c>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="25" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>298</v>
-      </c>
-      <c r="C5" s="32" t="s">
         <v>299</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="25" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>298</v>
-      </c>
-      <c r="C6" s="32" t="s">
-        <v>300</v>
+        <v>299</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="25" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>298</v>
-      </c>
-      <c r="C7" s="32" t="s">
-        <v>301</v>
+        <v>299</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="25" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>302</v>
-      </c>
-      <c r="C8" s="32" t="s">
         <v>303</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="25" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>302</v>
-      </c>
-      <c r="C9" s="32" t="s">
-        <v>305</v>
+        <v>303</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="25" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>306</v>
-      </c>
-      <c r="C10" s="32" t="s">
         <v>307</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="25" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>306</v>
-      </c>
-      <c r="C11" s="32" t="s">
-        <v>308</v>
+        <v>307</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="25" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>306</v>
-      </c>
-      <c r="C12" s="32" t="s">
-        <v>309</v>
+        <v>307</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="25" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>306</v>
-      </c>
-      <c r="C13" s="32" t="s">
-        <v>310</v>
+        <v>307</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="25" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>306</v>
-      </c>
-      <c r="C14" s="32" t="s">
-        <v>311</v>
+        <v>307</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="25" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>306</v>
-      </c>
-      <c r="C15" s="32" t="s">
-        <v>312</v>
+        <v>307</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="25" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>306</v>
-      </c>
-      <c r="C16" s="32" t="s">
-        <v>313</v>
+        <v>307</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="25" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>306</v>
-      </c>
-      <c r="C17" s="32" t="s">
-        <v>314</v>
+        <v>307</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="25" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>315</v>
-      </c>
-      <c r="C18" s="32" t="s">
         <v>316</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="25" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>315</v>
-      </c>
-      <c r="C19" s="32" t="s">
-        <v>317</v>
+        <v>316</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="25" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>315</v>
-      </c>
-      <c r="C20" s="32" t="s">
-        <v>318</v>
+        <v>316</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="25" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>315</v>
-      </c>
-      <c r="C21" s="32" t="s">
-        <v>319</v>
+        <v>316</v>
+      </c>
+      <c r="C21" s="31" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="25" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>315</v>
-      </c>
-      <c r="C22" s="32" t="s">
-        <v>320</v>
+        <v>316</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="25" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>315</v>
-      </c>
-      <c r="C23" s="32" t="s">
-        <v>321</v>
+        <v>316</v>
+      </c>
+      <c r="C23" s="31" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4179,74 +4001,74 @@
       <c r="B24" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="C24" s="32" t="s">
-        <v>322</v>
+      <c r="C24" s="31" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="25" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B25" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="C25" s="32" t="s">
-        <v>323</v>
+      <c r="C25" s="31" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="25" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B26" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="C26" s="32" t="s">
-        <v>324</v>
+      <c r="C26" s="31" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="25" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B27" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="C27" s="32" t="s">
-        <v>325</v>
+      <c r="C27" s="31" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="25" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B28" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="C28" s="32" t="s">
-        <v>326</v>
+      <c r="C28" s="31" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="25" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B29" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="C29" s="32" t="s">
-        <v>327</v>
+      <c r="C29" s="31" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="25" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B30" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="C30" s="32" t="s">
-        <v>328</v>
+      <c r="C30" s="31" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4254,65 +4076,65 @@
         <v>165</v>
       </c>
       <c r="B31" s="25" t="s">
-        <v>329</v>
-      </c>
-      <c r="C31" s="32" t="s">
         <v>330</v>
+      </c>
+      <c r="C31" s="31" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="25" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>329</v>
-      </c>
-      <c r="C32" s="32" t="s">
-        <v>331</v>
+        <v>330</v>
+      </c>
+      <c r="C32" s="31" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="25" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B33" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="C33" s="32" t="s">
-        <v>332</v>
+      <c r="C33" s="31" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="25" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B34" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="C34" s="32" t="s">
-        <v>333</v>
+      <c r="C34" s="31" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="25" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B35" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="C35" s="32" t="s">
-        <v>334</v>
+      <c r="C35" s="31" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="25" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B36" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="C36" s="32" t="s">
-        <v>335</v>
+      <c r="C36" s="31" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8183,7 +8005,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -8193,9 +8015,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.65234375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.51"/>
@@ -8206,21 +8028,21 @@
         <v>143</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>158</v>
@@ -8228,14 +8050,14 @@
       <c r="C2" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="D2" s="35"/>
+      <c r="D2" s="33"/>
       <c r="E2" s="1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>158</v>
@@ -8243,14 +8065,14 @@
       <c r="C3" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="35"/>
+      <c r="D3" s="33"/>
       <c r="E3" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>158</v>
@@ -8258,14 +8080,14 @@
       <c r="C4" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="D4" s="35"/>
+      <c r="D4" s="33"/>
       <c r="E4" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>158</v>
@@ -8273,14 +8095,14 @@
       <c r="C5" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="35"/>
+      <c r="D5" s="33"/>
       <c r="E5" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>159</v>
@@ -8288,14 +8110,14 @@
       <c r="C6" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="D6" s="35"/>
+      <c r="D6" s="33"/>
       <c r="E6" s="1" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>159</v>
@@ -8303,14 +8125,14 @@
       <c r="C7" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="D7" s="35"/>
+      <c r="D7" s="33"/>
       <c r="E7" s="1" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>159</v>
@@ -8318,14 +8140,14 @@
       <c r="C8" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="D8" s="35"/>
+      <c r="D8" s="33"/>
       <c r="E8" s="1" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>159</v>
@@ -8333,14 +8155,14 @@
       <c r="C9" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="D9" s="35"/>
+      <c r="D9" s="33"/>
       <c r="E9" s="1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>159</v>
@@ -8348,14 +8170,14 @@
       <c r="C10" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="D10" s="35"/>
-      <c r="E10" s="36" t="s">
-        <v>348</v>
+      <c r="D10" s="33"/>
+      <c r="E10" s="34" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>159</v>
@@ -8363,14 +8185,14 @@
       <c r="C11" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D11" s="35"/>
+      <c r="D11" s="33"/>
       <c r="E11" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>159</v>
@@ -8378,14 +8200,14 @@
       <c r="C12" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="D12" s="35"/>
+      <c r="D12" s="33"/>
       <c r="E12" s="1" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>159</v>
@@ -8393,9 +8215,9 @@
       <c r="C13" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="D13" s="35"/>
+      <c r="D13" s="33"/>
       <c r="E13" s="1" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📝 Agregar tilde a Bolívar
</commit_message>
<xml_diff>
--- a/aplicaciones/procesador/datos/Mapa 7ma - Datos.xlsx
+++ b/aplicaciones/procesador/datos/Mapa 7ma - Datos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -141,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="353">
   <si>
     <t xml:space="preserve">edificio los venados</t>
   </si>
@@ -260,7 +260,7 @@
     <t xml:space="preserve">criterio</t>
   </si>
   <si>
-    <t xml:space="preserve">Plaza Bolivar </t>
+    <t xml:space="preserve">Plaza de Bolívar</t>
   </si>
   <si>
     <t xml:space="preserve">avenida jiménez</t>
@@ -627,9 +627,6 @@
   </si>
   <si>
     <t xml:space="preserve">Texto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plaza de Bolívar</t>
   </si>
   <si>
     <t xml:space="preserve">0,53</t>
@@ -1610,15 +1607,15 @@
   </sheetPr>
   <dimension ref="A1:AR34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.65234375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.25"/>
@@ -1627,11 +1624,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="29.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="25.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="14.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="18.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="18.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="18.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="27.63"/>
@@ -1639,7 +1636,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="27.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="13.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="15.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="15.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="17.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="26.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="32.13"/>
@@ -1825,7 +1822,7 @@
       <c r="AQ4" s="5"/>
       <c r="AR4" s="4"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4"/>
       <c r="B5" s="4" t="s">
         <v>38</v>
@@ -2415,13 +2412,13 @@
   </sheetPr>
   <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="R2" activeCellId="0" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.65234375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.63"/>
@@ -2429,7 +2426,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.51"/>
@@ -2437,7 +2434,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="15.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="40.88"/>
@@ -2508,7 +2505,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>162</v>
+        <v>39</v>
       </c>
       <c r="C2" s="23" t="n">
         <v>4.59779533018865</v>
@@ -2517,16 +2514,16 @@
         <v>-74.0756536703986</v>
       </c>
       <c r="E2" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="M2" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="M2" s="25" t="s">
+      <c r="N2" s="25" t="s">
         <v>164</v>
       </c>
-      <c r="N2" s="25" t="s">
+      <c r="R2" s="0" t="s">
         <v>165</v>
-      </c>
-      <c r="R2" s="0" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2534,7 +2531,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C3" s="23" t="n">
         <v>4.601444</v>
@@ -2544,19 +2541,19 @@
       </c>
       <c r="E3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="R3" s="27" t="s">
         <v>170</v>
-      </c>
-      <c r="R3" s="27" t="s">
-        <v>171</v>
       </c>
       <c r="S3" s="27"/>
     </row>
@@ -2565,7 +2562,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C4" s="23" t="n">
         <v>4.605297</v>
@@ -2574,19 +2571,19 @@
         <v>-74.071588</v>
       </c>
       <c r="E4" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>175</v>
       </c>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="Q4" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2594,7 +2591,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C5" s="23" t="n">
         <v>4.61134</v>
@@ -2603,10 +2600,10 @@
         <v>-74.069874</v>
       </c>
       <c r="E5" s="24" t="s">
+        <v>177</v>
+      </c>
+      <c r="I5" s="25" t="s">
         <v>178</v>
-      </c>
-      <c r="I5" s="25" t="s">
-        <v>179</v>
       </c>
       <c r="J5" s="25"/>
       <c r="K5" s="25"/>
@@ -2624,7 +2621,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C6" s="23" t="n">
         <v>4.618599</v>
@@ -2633,10 +2630,10 @@
         <v>-74.068069</v>
       </c>
       <c r="E6" s="24" t="s">
+        <v>177</v>
+      </c>
+      <c r="I6" s="25" t="s">
         <v>178</v>
-      </c>
-      <c r="I6" s="25" t="s">
-        <v>179</v>
       </c>
       <c r="J6" s="25"/>
       <c r="K6" s="25"/>
@@ -2645,13 +2642,13 @@
       <c r="N6" s="25"/>
       <c r="O6" s="25"/>
       <c r="P6" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q6" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="R6" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="S6" s="1"/>
     </row>
@@ -2660,7 +2657,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C7" s="23" t="n">
         <v>4.62475</v>
@@ -2669,13 +2666,13 @@
         <v>-74.066423</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F7" s="28" t="n">
         <v>1</v>
       </c>
       <c r="I7" s="25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J7" s="25"/>
       <c r="K7" s="25"/>
@@ -2684,7 +2681,7 @@
       <c r="N7" s="25"/>
       <c r="O7" s="25"/>
       <c r="R7" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="S7" s="1"/>
     </row>
@@ -2702,21 +2699,21 @@
         <v>-74.064257</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I8" s="25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J8" s="25"/>
       <c r="K8" s="25"/>
       <c r="L8" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M8" s="25"/>
       <c r="N8" s="25"/>
       <c r="O8" s="25"/>
       <c r="R8" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="S8" s="1"/>
     </row>
@@ -2725,7 +2722,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C9" s="23" t="n">
         <v>4.6282521</v>
@@ -2734,17 +2731,17 @@
         <v>-74.0670904</v>
       </c>
       <c r="E9" s="24" t="s">
+        <v>189</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>192</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -2755,7 +2752,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C10" s="23" t="n">
         <v>4.639489</v>
@@ -2764,24 +2761,24 @@
         <v>-74.062897</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F10" s="28" t="n">
         <v>2</v>
       </c>
       <c r="G10" s="28" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="M10" s="25" t="s">
         <v>197</v>
-      </c>
-      <c r="M10" s="25" t="s">
-        <v>198</v>
       </c>
       <c r="N10" s="25"/>
       <c r="O10" s="25"/>
@@ -2791,7 +2788,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C11" s="23" t="n">
         <v>4.641975</v>
@@ -2800,13 +2797,13 @@
         <v>-74.062267</v>
       </c>
       <c r="E11" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="H11" s="25" t="s">
         <v>200</v>
       </c>
-      <c r="H11" s="25" t="s">
-        <v>201</v>
-      </c>
       <c r="I11" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -2820,7 +2817,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C12" s="23" t="n">
         <v>4.645357</v>
@@ -2829,40 +2826,40 @@
         <v>-74.061291</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F12" s="28" t="n">
         <v>3</v>
       </c>
       <c r="G12" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>205</v>
-      </c>
       <c r="I12" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="N12" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="N12" s="1" t="s">
+      <c r="O12" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="O12" s="1" t="s">
+      <c r="P12" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="P12" s="1" t="s">
+      <c r="Q12" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="Q12" s="1" t="s">
+      <c r="R12" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>211</v>
       </c>
       <c r="S12" s="1"/>
     </row>
@@ -2871,7 +2868,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C13" s="23" t="n">
         <v>4.6507</v>
@@ -2880,10 +2877,10 @@
         <v>-74.05822</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -2891,10 +2888,10 @@
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2902,7 +2899,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C14" s="23" t="n">
         <v>4.652758</v>
@@ -2911,10 +2908,10 @@
         <v>-74.056551</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -2923,7 +2920,7 @@
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2931,7 +2928,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C15" s="23" t="n">
         <v>4.65487400724876</v>
@@ -2940,10 +2937,10 @@
         <v>-74.0554333681108</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -2952,10 +2949,10 @@
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="S15" s="1"/>
     </row>
@@ -2964,7 +2961,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C16" s="23" t="n">
         <v>4.65671780613089</v>
@@ -2973,10 +2970,10 @@
         <v>-74.0543665308446</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -2990,7 +2987,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C17" s="23" t="n">
         <v>4.65869671902702</v>
@@ -2999,16 +2996,16 @@
         <v>-74.0527981659214</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="N17" s="25"/>
       <c r="O17" s="25"/>
@@ -3018,7 +3015,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C18" s="23" t="n">
         <v>4.66306901162081</v>
@@ -3027,27 +3024,27 @@
         <v>-74.0486994996409</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G18" s="28" t="s">
+        <v>223</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>225</v>
-      </c>
       <c r="I18" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
       <c r="R18" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="S18" s="1"/>
     </row>
@@ -3056,7 +3053,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C19" s="23" t="n">
         <v>4.66516565077258</v>
@@ -3065,13 +3062,13 @@
         <v>-74.0468160288417</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F19" s="28" t="n">
         <v>4</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
@@ -3081,7 +3078,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C20" s="23" t="n">
         <v>4.67138521212362</v>
@@ -3090,10 +3087,10 @@
         <v>-74.0438000439461</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -3102,7 +3099,7 @@
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="R20" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="S20" s="1"/>
     </row>
@@ -3111,7 +3108,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C21" s="23" t="n">
         <v>4.67447260123109</v>
@@ -3120,10 +3117,10 @@
         <v>-74.0417018437693</v>
       </c>
       <c r="E21" s="24" t="s">
+        <v>189</v>
+      </c>
+      <c r="I21" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>191</v>
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -3132,7 +3129,7 @@
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="R21" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="S21" s="1"/>
     </row>
@@ -3141,7 +3138,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C22" s="23" t="n">
         <v>4.67985737530602</v>
@@ -3150,10 +3147,10 @@
         <v>-74.0382125791768</v>
       </c>
       <c r="E22" s="24" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -3162,10 +3159,10 @@
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="Q22" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="Q22" s="1" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3173,7 +3170,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C23" s="23" t="n">
         <v>4.6851414298036</v>
@@ -3182,16 +3179,16 @@
         <v>-74.0356604991655</v>
       </c>
       <c r="E23" s="24" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F23" s="28" t="n">
         <v>5</v>
       </c>
       <c r="G23" s="28" t="s">
+        <v>237</v>
+      </c>
+      <c r="I23" s="25" t="s">
         <v>238</v>
-      </c>
-      <c r="I23" s="25" t="s">
-        <v>239</v>
       </c>
       <c r="J23" s="25"/>
       <c r="K23" s="25"/>
@@ -3200,7 +3197,7 @@
       <c r="N23" s="25"/>
       <c r="O23" s="25"/>
       <c r="R23" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="S23" s="1"/>
     </row>
@@ -3209,7 +3206,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C24" s="23" t="n">
         <v>4.69366275843025</v>
@@ -3218,10 +3215,10 @@
         <v>-74.0332252216773</v>
       </c>
       <c r="E24" s="24" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I24" s="25" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J24" s="25"/>
       <c r="K24" s="25"/>
@@ -3230,7 +3227,7 @@
       <c r="N24" s="25"/>
       <c r="O24" s="25"/>
       <c r="R24" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="S24" s="1"/>
     </row>
@@ -3239,7 +3236,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C25" s="23" t="n">
         <v>4.70213634871971</v>
@@ -3248,10 +3245,10 @@
         <v>-74.0285922020549</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I25" s="25" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J25" s="25"/>
       <c r="K25" s="25"/>
@@ -3265,7 +3262,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C26" s="23" t="n">
         <v>4.71168163739051</v>
@@ -3274,16 +3271,16 @@
         <v>-74.029166381959</v>
       </c>
       <c r="E26" s="24" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F26" s="28" t="n">
         <v>6</v>
       </c>
       <c r="G26" s="28" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I26" s="25" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J26" s="25"/>
       <c r="K26" s="25"/>
@@ -3297,7 +3294,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C27" s="23" t="n">
         <v>4.71618941013746</v>
@@ -3306,21 +3303,21 @@
         <v>-74.028746372056</v>
       </c>
       <c r="E27" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I27" s="25" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J27" s="25"/>
       <c r="K27" s="25"/>
       <c r="L27" s="25"/>
       <c r="M27" s="25" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N27" s="25"/>
       <c r="O27" s="25"/>
       <c r="R27" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="S27" s="1"/>
     </row>
@@ -3329,7 +3326,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C28" s="23" t="n">
         <v>4.72271112809495</v>
@@ -3338,10 +3335,10 @@
         <v>-74.0261459774934</v>
       </c>
       <c r="E28" s="24" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I28" s="25" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J28" s="25"/>
       <c r="K28" s="25"/>
@@ -3355,7 +3352,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C29" s="23" t="n">
         <v>4.72561860463364</v>
@@ -3364,10 +3361,10 @@
         <v>-74.0248846037107</v>
       </c>
       <c r="E29" s="24" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I29" s="25" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J29" s="25"/>
       <c r="K29" s="25"/>
@@ -3376,7 +3373,7 @@
       <c r="N29" s="25"/>
       <c r="O29" s="25"/>
       <c r="Q29" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3384,7 +3381,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C30" s="23" t="n">
         <v>4.72759203191308</v>
@@ -3393,13 +3390,13 @@
         <v>-74.0246188787511</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I30" s="25" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J30" s="25"/>
       <c r="K30" s="25"/>
@@ -3413,7 +3410,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C31" s="23" t="n">
         <v>4.73504479371492</v>
@@ -3422,24 +3419,24 @@
         <v>-74.0243405599811</v>
       </c>
       <c r="E31" s="24" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G31" s="28" t="s">
+        <v>256</v>
+      </c>
+      <c r="H31" s="25" t="s">
         <v>257</v>
       </c>
-      <c r="H31" s="25" t="s">
-        <v>258</v>
-      </c>
       <c r="I31" s="25" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J31" s="25"/>
       <c r="K31" s="25"/>
       <c r="L31" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="M31" s="1" t="s">
         <v>259</v>
-      </c>
-      <c r="M31" s="1" t="s">
-        <v>260</v>
       </c>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
@@ -3449,7 +3446,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C32" s="23" t="n">
         <v>4.73928285919624</v>
@@ -3458,10 +3455,10 @@
         <v>-74.0227685844767</v>
       </c>
       <c r="E32" s="24" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
@@ -3472,7 +3469,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C33" s="23" t="n">
         <v>4.74104500723192</v>
@@ -3481,13 +3478,13 @@
         <v>-74.0223245655917</v>
       </c>
       <c r="E33" s="24" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H33" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="R33" s="1" t="s">
         <v>264</v>
-      </c>
-      <c r="R33" s="1" t="s">
-        <v>265</v>
       </c>
       <c r="S33" s="1"/>
     </row>
@@ -3496,7 +3493,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="28" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C34" s="23" t="n">
         <v>4.74704550134667</v>
@@ -3505,23 +3502,23 @@
         <v>-74.0226372775582</v>
       </c>
       <c r="E34" s="24" t="s">
+        <v>266</v>
+      </c>
+      <c r="G34" s="28" t="s">
         <v>267</v>
       </c>
-      <c r="G34" s="28" t="s">
+      <c r="J34" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="J34" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="K34" s="1"/>
       <c r="L34" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
       <c r="P34" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3529,7 +3526,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C35" s="23" t="n">
         <v>4.75396347261005</v>
@@ -3538,10 +3535,10 @@
         <v>-74.0244240661433</v>
       </c>
       <c r="E35" s="24" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q35" s="1" t="s">
         <v>273</v>
-      </c>
-      <c r="Q35" s="1" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3549,7 +3546,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C36" s="23" t="n">
         <v>4.75617544590708</v>
@@ -3558,13 +3555,13 @@
         <v>-74.0246792916686</v>
       </c>
       <c r="E36" s="24" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="Q36" s="29" t="s">
+        <v>275</v>
+      </c>
+      <c r="R36" s="1" t="s">
         <v>276</v>
-      </c>
-      <c r="R36" s="1" t="s">
-        <v>277</v>
       </c>
       <c r="S36" s="1"/>
     </row>
@@ -3573,7 +3570,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C37" s="23" t="n">
         <v>4.76052434895997</v>
@@ -3582,10 +3579,10 @@
         <v>-74.0263419552712</v>
       </c>
       <c r="E37" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="R37" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="S37" s="1"/>
     </row>
@@ -3594,7 +3591,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="28" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C38" s="23" t="n">
         <v>4.76566235110988</v>
@@ -3603,13 +3600,13 @@
         <v>-74.027549403371</v>
       </c>
       <c r="E38" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G38" s="28" t="s">
+        <v>280</v>
+      </c>
+      <c r="O38" s="1" t="s">
         <v>281</v>
-      </c>
-      <c r="O38" s="1" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3617,7 +3614,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C39" s="23" t="n">
         <v>4.7689779473818</v>
@@ -3626,7 +3623,7 @@
         <v>-74.0273381986581</v>
       </c>
       <c r="E39" s="24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3634,7 +3631,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C40" s="23" t="n">
         <v>4.76966052997788</v>
@@ -3643,10 +3640,10 @@
         <v>-74.0270269840824</v>
       </c>
       <c r="E40" s="24" t="s">
+        <v>285</v>
+      </c>
+      <c r="R40" s="1" t="s">
         <v>286</v>
-      </c>
-      <c r="R40" s="1" t="s">
-        <v>287</v>
       </c>
       <c r="S40" s="1"/>
     </row>
@@ -3655,7 +3652,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C41" s="23" t="n">
         <v>4.7771118817951</v>
@@ -3664,10 +3661,10 @@
         <v>-74.0260495949368</v>
       </c>
       <c r="E41" s="24" t="s">
+        <v>288</v>
+      </c>
+      <c r="R41" s="1" t="s">
         <v>289</v>
-      </c>
-      <c r="R41" s="1" t="s">
-        <v>290</v>
       </c>
       <c r="S41" s="1"/>
     </row>
@@ -3676,7 +3673,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C42" s="23" t="n">
         <v>4.79861514914944</v>
@@ -3685,7 +3682,7 @@
         <v>-74.0307002114146</v>
       </c>
       <c r="E42" s="24" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -3710,7 +3707,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.65234375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.62"/>
@@ -3722,21 +3719,21 @@
         <v>143</v>
       </c>
       <c r="B1" s="30" t="s">
+        <v>292</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>293</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B2" s="25" t="s">
+        <v>294</v>
+      </c>
+      <c r="C2" s="31" t="s">
         <v>295</v>
-      </c>
-      <c r="C2" s="31" t="s">
-        <v>296</v>
       </c>
       <c r="D2" s="31"/>
       <c r="E2" s="31"/>
@@ -3744,13 +3741,13 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D3" s="32"/>
       <c r="E3" s="32"/>
@@ -3768,13 +3765,13 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="25" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D4" s="16"/>
       <c r="E4" s="16"/>
@@ -3787,354 +3784,354 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="25" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B5" s="25" t="s">
+        <v>298</v>
+      </c>
+      <c r="C5" s="31" t="s">
         <v>299</v>
-      </c>
-      <c r="C5" s="31" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="25" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="25" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="25" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B8" s="25" t="s">
+        <v>302</v>
+      </c>
+      <c r="C8" s="31" t="s">
         <v>303</v>
-      </c>
-      <c r="C8" s="31" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="25" t="s">
+        <v>304</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>302</v>
+      </c>
+      <c r="C9" s="31" t="s">
         <v>305</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>303</v>
-      </c>
-      <c r="C9" s="31" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="25" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B10" s="25" t="s">
+        <v>306</v>
+      </c>
+      <c r="C10" s="31" t="s">
         <v>307</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="25" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="25" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="25" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="25" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B18" s="25" t="s">
+        <v>315</v>
+      </c>
+      <c r="C18" s="31" t="s">
         <v>316</v>
-      </c>
-      <c r="C18" s="31" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="25" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="25" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="25" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="25" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B24" s="25" t="s">
         <v>147</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="25" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B25" s="25" t="s">
         <v>147</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="25" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B26" s="25" t="s">
         <v>147</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="25" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B27" s="25" t="s">
         <v>147</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B28" s="25" t="s">
         <v>147</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="25" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B29" s="25" t="s">
         <v>147</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="25" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B30" s="25" t="s">
         <v>147</v>
       </c>
       <c r="C30" s="31" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B31" s="25" t="s">
+        <v>329</v>
+      </c>
+      <c r="C31" s="31" t="s">
         <v>330</v>
-      </c>
-      <c r="C31" s="31" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B33" s="25" t="s">
         <v>119</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B34" s="25" t="s">
         <v>119</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="25" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B35" s="25" t="s">
         <v>119</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="25" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B36" s="25" t="s">
         <v>119</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8015,7 +8012,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.65234375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.75"/>
@@ -8028,21 +8025,21 @@
         <v>143</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>339</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>158</v>
@@ -8052,12 +8049,12 @@
       </c>
       <c r="D2" s="33"/>
       <c r="E2" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>158</v>
@@ -8067,12 +8064,12 @@
       </c>
       <c r="D3" s="33"/>
       <c r="E3" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>158</v>
@@ -8082,12 +8079,12 @@
       </c>
       <c r="D4" s="33"/>
       <c r="E4" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>158</v>
@@ -8097,12 +8094,12 @@
       </c>
       <c r="D5" s="33"/>
       <c r="E5" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>159</v>
@@ -8112,12 +8109,12 @@
       </c>
       <c r="D6" s="33"/>
       <c r="E6" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>159</v>
@@ -8127,12 +8124,12 @@
       </c>
       <c r="D7" s="33"/>
       <c r="E7" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>159</v>
@@ -8142,12 +8139,12 @@
       </c>
       <c r="D8" s="33"/>
       <c r="E8" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>159</v>
@@ -8157,12 +8154,12 @@
       </c>
       <c r="D9" s="33"/>
       <c r="E9" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>159</v>
@@ -8172,12 +8169,12 @@
       </c>
       <c r="D10" s="33"/>
       <c r="E10" s="34" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>159</v>
@@ -8187,12 +8184,12 @@
       </c>
       <c r="D11" s="33"/>
       <c r="E11" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>159</v>
@@ -8202,12 +8199,12 @@
       </c>
       <c r="D12" s="33"/>
       <c r="E12" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>159</v>
@@ -8217,7 +8214,7 @@
       </c>
       <c r="D13" s="33"/>
       <c r="E13" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
🎨  Agregar fondos e ilustraciones
</commit_message>
<xml_diff>
--- a/aplicaciones/procesador/datos/Mapa 7ma - Datos.xlsx
+++ b/aplicaciones/procesador/datos/Mapa 7ma - Datos.xlsx
@@ -1612,10 +1612,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="L1" activeCellId="0" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C5" activeCellId="1" sqref="R20 C5"/>
+      <selection pane="bottomRight" activeCell="C5" activeCellId="1" sqref="R15 C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.70703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.25"/>
@@ -2413,12 +2413,12 @@
   <dimension ref="A1:S42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="R20" activeCellId="0" sqref="R20"/>
+      <selection pane="bottomLeft" activeCell="R15" activeCellId="0" sqref="R15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.70703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.63"/>
@@ -2924,7 +2924,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="26" t="n">
         <v>14</v>
       </c>
@@ -2957,7 +2957,7 @@
       </c>
       <c r="S15" s="1"/>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>15</v>
       </c>
@@ -3522,7 +3522,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="26" t="n">
         <v>34</v>
       </c>
@@ -3705,10 +3705,10 @@
   <dimension ref="A1:P1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="R20 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="R15 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.70703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.62"/>
@@ -8010,10 +8010,10 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="R20 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="R15 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.70703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.75"/>

</xml_diff>

<commit_message>
📝 Mostrar nombres de lugares al pasar el ratón por encima
</commit_message>
<xml_diff>
--- a/aplicaciones/procesador/datos/Mapa 7ma - Datos.xlsx
+++ b/aplicaciones/procesador/datos/Mapa 7ma - Datos.xlsx
@@ -638,9 +638,6 @@
     <t xml:space="preserve">tfp1</t>
   </si>
   <si>
-    <t xml:space="preserve">plaza_de_bolivar</t>
-  </si>
-  <si>
     <t xml:space="preserve">Avenida Jiménez</t>
   </si>
   <si>
@@ -653,7 +650,7 @@
     <t xml:space="preserve">tsa1</t>
   </si>
   <si>
-    <t xml:space="preserve">iglesia_san_francisco</t>
+    <t xml:space="preserve">Iglesia San Francisco</t>
   </si>
   <si>
     <t xml:space="preserve">Calle 19</t>
@@ -680,6 +677,9 @@
     <t xml:space="preserve">tpj1</t>
   </si>
   <si>
+    <t xml:space="preserve">Planetario de Bogotá</t>
+  </si>
+  <si>
     <t xml:space="preserve">Calle 32</t>
   </si>
   <si>
@@ -695,13 +695,13 @@
     <t xml:space="preserve">0,6</t>
   </si>
   <si>
-    <t xml:space="preserve">parque_nacional</t>
+    <t xml:space="preserve">Parque Nacional</t>
   </si>
   <si>
     <t xml:space="preserve">tca2</t>
   </si>
   <si>
-    <t xml:space="preserve">universidad_javeriana</t>
+    <t xml:space="preserve">Universidad Javeriana</t>
   </si>
   <si>
     <t xml:space="preserve">Calle 45</t>
@@ -770,7 +770,7 @@
     <t xml:space="preserve">pe4</t>
   </si>
   <si>
-    <t xml:space="preserve">parque_hippies</t>
+    <t xml:space="preserve">Parque de los Hippies</t>
   </si>
   <si>
     <t xml:space="preserve">Calle 67</t>
@@ -782,7 +782,7 @@
     <t xml:space="preserve">tsa3</t>
   </si>
   <si>
-    <t xml:space="preserve">edificio_caracol</t>
+    <t xml:space="preserve">Edificio Caracol</t>
   </si>
   <si>
     <t xml:space="preserve">Calle 70</t>
@@ -794,7 +794,7 @@
     <t xml:space="preserve">0,58</t>
   </si>
   <si>
-    <t xml:space="preserve">edificio_venados</t>
+    <t xml:space="preserve">Edificio Los Venados</t>
   </si>
   <si>
     <t xml:space="preserve">Calle 74</t>
@@ -821,7 +821,7 @@
     <t xml:space="preserve">tca5</t>
   </si>
   <si>
-    <t xml:space="preserve">subida_patios</t>
+    <t xml:space="preserve">Subida a Patios</t>
   </si>
   <si>
     <t xml:space="preserve">Calle 85</t>
@@ -833,7 +833,7 @@
     <t xml:space="preserve">0,5</t>
   </si>
   <si>
-    <t xml:space="preserve">museo_del_chico</t>
+    <t xml:space="preserve">Museo del Chicó</t>
   </si>
   <si>
     <t xml:space="preserve">Calle 94</t>
@@ -848,7 +848,7 @@
     <t xml:space="preserve">pe7</t>
   </si>
   <si>
-    <t xml:space="preserve">seminario_conciliar</t>
+    <t xml:space="preserve">Seminario Conciliar</t>
   </si>
   <si>
     <t xml:space="preserve">Calle 106</t>
@@ -860,7 +860,7 @@
     <t xml:space="preserve">tpj3</t>
   </si>
   <si>
-    <t xml:space="preserve">escuela_caballeria</t>
+    <t xml:space="preserve">Escuela de Caballería</t>
   </si>
   <si>
     <t xml:space="preserve">Calle 116</t>
@@ -869,7 +869,7 @@
     <t xml:space="preserve">0,68</t>
   </si>
   <si>
-    <t xml:space="preserve">hacienda_santa_barbara</t>
+    <t xml:space="preserve">Hacienda Santa Bárbara</t>
   </si>
   <si>
     <t xml:space="preserve">Calle 127</t>
@@ -887,7 +887,7 @@
     <t xml:space="preserve">tcm6</t>
   </si>
   <si>
-    <t xml:space="preserve">centro_comercial_palatino</t>
+    <t xml:space="preserve">Centro Comercial Palatino</t>
   </si>
   <si>
     <t xml:space="preserve">Calle 147</t>
@@ -935,7 +935,7 @@
     <t xml:space="preserve">t15m6</t>
   </si>
   <si>
-    <t xml:space="preserve">hospital_simon_bolivar</t>
+    <t xml:space="preserve">Hospital Simón Bolívar</t>
   </si>
   <si>
     <t xml:space="preserve">Calle 170</t>
@@ -971,13 +971,13 @@
     <t xml:space="preserve">pe5</t>
   </si>
   <si>
-    <t xml:space="preserve">abastos_codabas</t>
+    <t xml:space="preserve">Abasto Codabas</t>
   </si>
   <si>
     <t xml:space="preserve">Calle 183</t>
   </si>
   <si>
-    <t xml:space="preserve">barrio_el_codito</t>
+    <t xml:space="preserve">Barrio El Codito</t>
   </si>
   <si>
     <t xml:space="preserve">Calle 189</t>
@@ -1001,7 +1001,7 @@
     <t xml:space="preserve">0,35</t>
   </si>
   <si>
-    <t xml:space="preserve">finca_la_suiza</t>
+    <t xml:space="preserve">Finca La Suiza</t>
   </si>
   <si>
     <t xml:space="preserve">Calle 200</t>
@@ -1010,7 +1010,7 @@
     <t xml:space="preserve">0,37</t>
   </si>
   <si>
-    <t xml:space="preserve">subestacion_torca</t>
+    <t xml:space="preserve">Subestación Torca</t>
   </si>
   <si>
     <t xml:space="preserve">Calle 220</t>
@@ -1612,7 +1612,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="L1" activeCellId="0" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C5" activeCellId="1" sqref="R15 C5"/>
+      <selection pane="bottomRight" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.70703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2413,9 +2413,9 @@
   <dimension ref="A1:S42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="R15" activeCellId="0" sqref="R15"/>
+      <selection pane="bottomLeft" activeCell="R12" activeCellId="0" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.70703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2523,7 +2523,7 @@
         <v>164</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>165</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2531,7 +2531,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C3" s="23" t="n">
         <v>4.601444</v>
@@ -2541,19 +2541,19 @@
       </c>
       <c r="E3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="R3" s="27" t="s">
         <v>169</v>
-      </c>
-      <c r="R3" s="27" t="s">
-        <v>170</v>
       </c>
       <c r="S3" s="27"/>
     </row>
@@ -2562,7 +2562,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C4" s="23" t="n">
         <v>4.605297</v>
@@ -2571,19 +2571,19 @@
         <v>-74.071588</v>
       </c>
       <c r="E4" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>174</v>
       </c>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="Q4" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2591,7 +2591,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C5" s="23" t="n">
         <v>4.61134</v>
@@ -2600,10 +2600,10 @@
         <v>-74.069874</v>
       </c>
       <c r="E5" s="24" t="s">
+        <v>176</v>
+      </c>
+      <c r="I5" s="25" t="s">
         <v>177</v>
-      </c>
-      <c r="I5" s="25" t="s">
-        <v>178</v>
       </c>
       <c r="J5" s="25"/>
       <c r="K5" s="25"/>
@@ -2612,7 +2612,7 @@
       <c r="N5" s="25"/>
       <c r="O5" s="25"/>
       <c r="R5" s="1" t="s">
-        <v>8</v>
+        <v>178</v>
       </c>
       <c r="S5" s="1"/>
     </row>
@@ -2630,10 +2630,10 @@
         <v>-74.068069</v>
       </c>
       <c r="E6" s="24" t="s">
+        <v>176</v>
+      </c>
+      <c r="I6" s="25" t="s">
         <v>177</v>
-      </c>
-      <c r="I6" s="25" t="s">
-        <v>178</v>
       </c>
       <c r="J6" s="25"/>
       <c r="K6" s="25"/>
@@ -2670,7 +2670,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="25" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J7" s="25"/>
       <c r="K7" s="25"/>
@@ -2700,7 +2700,7 @@
         <v>183</v>
       </c>
       <c r="I8" s="25" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J8" s="25"/>
       <c r="K8" s="25"/>
@@ -3420,7 +3420,7 @@
         <v>-74.0243405599811</v>
       </c>
       <c r="E31" s="24" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G31" s="28" t="s">
         <v>256</v>
@@ -3479,7 +3479,7 @@
         <v>-74.0223245655917</v>
       </c>
       <c r="E33" s="24" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>263</v>
@@ -3705,7 +3705,7 @@
   <dimension ref="A1:P1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="R15 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.70703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3728,7 +3728,7 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>294</v>
@@ -3785,7 +3785,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B5" s="25" t="s">
         <v>298</v>
@@ -3818,7 +3818,7 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B8" s="25" t="s">
         <v>302</v>
@@ -3840,7 +3840,7 @@
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="25" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B10" s="25" t="s">
         <v>306</v>
@@ -4005,7 +4005,7 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="25" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B25" s="25" t="s">
         <v>147</v>
@@ -4093,7 +4093,7 @@
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="25" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B33" s="25" t="s">
         <v>119</v>
@@ -8010,7 +8010,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="R15 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.70703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8175,7 +8175,7 @@
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>159</v>

</xml_diff>

<commit_message>
🐛 Arreglar lugares e ilustraciones
</commit_message>
<xml_diff>
--- a/aplicaciones/procesador/datos/Mapa 7ma - Datos.xlsx
+++ b/aplicaciones/procesador/datos/Mapa 7ma - Datos.xlsx
@@ -971,7 +971,7 @@
     <t xml:space="preserve">pe5</t>
   </si>
   <si>
-    <t xml:space="preserve">Abasto Codabas</t>
+    <t xml:space="preserve">Centro de abastos Codabas</t>
   </si>
   <si>
     <t xml:space="preserve">Calle 183</t>
@@ -1608,11 +1608,11 @@
   <dimension ref="A1:AR34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="L6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="AR6" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="topRight" activeCell="AR1" activeCellId="0" sqref="AR1"/>
       <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="C5" activeCellId="1" sqref="R36 C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.70703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2413,9 +2413,9 @@
   <dimension ref="A1:S42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="R12" activeCellId="0" sqref="R12"/>
+      <selection pane="bottomLeft" activeCell="R36" activeCellId="0" sqref="R36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.70703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3705,7 +3705,7 @@
   <dimension ref="A1:P1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="R36 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.70703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8010,7 +8010,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="R36 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.70703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
⚡️ Agregar textos pájaros
</commit_message>
<xml_diff>
--- a/aplicaciones/procesador/datos/Mapa 7ma - Datos.xlsx
+++ b/aplicaciones/procesador/datos/Mapa 7ma - Datos.xlsx
@@ -596,7 +596,7 @@
     <t xml:space="preserve">Txt 15 minutos </t>
   </si>
   <si>
-    <t xml:space="preserve">Txt Pájaros</t>
+    <t xml:space="preserve">txtPajaros</t>
   </si>
   <si>
     <t xml:space="preserve">Txt Basuras</t>
@@ -1612,10 +1612,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="AR1" activeCellId="0" sqref="AR1"/>
       <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C5" activeCellId="1" sqref="R36 C5"/>
+      <selection pane="bottomRight" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.70703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.72265625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.25"/>
@@ -2415,10 +2415,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="R36" activeCellId="0" sqref="R36"/>
+      <selection pane="bottomLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.70703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.72265625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.63"/>
@@ -3705,10 +3705,10 @@
   <dimension ref="A1:P1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="R36 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.70703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.72265625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.62"/>
@@ -8010,10 +8010,10 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="R36 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.70703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.72265625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.75"/>

</xml_diff>

<commit_message>
📝 Dejar un solo podcast por punto en datos (dejé una copia del original por si acaso)
</commit_message>
<xml_diff>
--- a/aplicaciones/procesador/datos/Mapa 7ma - Datos.xlsx
+++ b/aplicaciones/procesador/datos/Mapa 7ma - Datos.xlsx
@@ -141,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="353">
   <si>
     <t xml:space="preserve">edificio los venados</t>
   </si>
@@ -764,22 +764,22 @@
     <t xml:space="preserve">tsa2</t>
   </si>
   <si>
+    <t xml:space="preserve">pe4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parque de los Hippies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calle 67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tsa3</t>
+  </si>
+  <si>
     <t xml:space="preserve">pd2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pe4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parque de los Hippies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calle 67</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,57</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tsa3</t>
   </si>
   <si>
     <t xml:space="preserve">Edificio Caracol</t>
@@ -1615,7 +1615,7 @@
       <selection pane="bottomRight" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.72265625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.25"/>
@@ -2413,12 +2413,12 @@
   <dimension ref="A1:S42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
+      <selection pane="bottomLeft" activeCell="P19" activeCellId="0" sqref="P19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.72265625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.63"/>
@@ -2850,14 +2850,12 @@
       <c r="O12" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="P12" s="1" t="s">
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="Q12" s="1" t="s">
+      <c r="R12" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="S12" s="1"/>
     </row>
@@ -2866,7 +2864,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C13" s="23" t="n">
         <v>4.6507</v>
@@ -2875,7 +2873,7 @@
         <v>-74.05822</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>189</v>
@@ -2886,16 +2884,16 @@
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="P13" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>207</v>
       </c>
       <c r="R13" s="0" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>13</v>
       </c>
@@ -2920,9 +2918,7 @@
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
-      <c r="P14" s="1" t="s">
-        <v>207</v>
-      </c>
+      <c r="P14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="26" t="n">
@@ -2949,9 +2945,7 @@
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
-      <c r="P15" s="1" t="s">
-        <v>207</v>
-      </c>
+      <c r="P15" s="1"/>
       <c r="R15" s="1" t="s">
         <v>217</v>
       </c>
@@ -3304,7 +3298,7 @@
         <v>-74.028746372056</v>
       </c>
       <c r="E27" s="24" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I27" s="25" t="s">
         <v>238</v>
@@ -3580,7 +3574,7 @@
         <v>-74.0263419552712</v>
       </c>
       <c r="E37" s="24" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="R37" s="1" t="s">
         <v>278</v>
@@ -3708,7 +3702,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.72265625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.62"/>
@@ -4115,7 +4109,7 @@
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="25" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B35" s="25" t="s">
         <v>119</v>
@@ -8013,7 +8007,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.72265625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.75"/>
@@ -8055,7 +8049,7 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>158</v>
@@ -8145,7 +8139,7 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>159</v>

</xml_diff>